<commit_message>
fix: town location scaling on devices
</commit_message>
<xml_diff>
--- a/data/welsh word/WelshWords_mega_sheet.xlsx
+++ b/data/welsh word/WelshWords_mega_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LZ986KT\Documents\1000-words\data\welsh word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E5887D4-71E3-450E-BD56-7AA7467B9972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D22199-122D-4B83-B6A5-73D7A1CD1BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2516" uniqueCount="1560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2517" uniqueCount="1561">
   <si>
     <t>Welsh</t>
   </si>
@@ -4720,6 +4720,9 @@
   </si>
   <si>
     <t>The Great Orme Copper Mines</t>
+  </si>
+  <si>
+    <t>cwtch</t>
   </si>
 </sst>
 </file>
@@ -4795,7 +4798,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -17422,10 +17425,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17882,6 +17885,11 @@
         <v>1557</v>
       </c>
     </row>
+    <row r="38" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J38" t="s">
+        <v>1560</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
fix: algorithm and data structure
</commit_message>
<xml_diff>
--- a/data/welsh word/WelshWords_mega_sheet.xlsx
+++ b/data/welsh word/WelshWords_mega_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LZ986KT\Documents\1000-words\data\welsh word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D22199-122D-4B83-B6A5-73D7A1CD1BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE54B67-36C1-429E-A305-7FBE3AF5D72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4722,7 +4722,7 @@
     <t>The Great Orme Copper Mines</t>
   </si>
   <si>
-    <t>cwtch</t>
+    <t>Cwtch</t>
   </si>
 </sst>
 </file>
@@ -17425,10 +17425,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17768,6 +17768,9 @@
       <c r="I20" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="K20" t="s">
+        <v>1560</v>
+      </c>
       <c r="L20">
         <f>COUNTIF(WelshWords_mega_sheet!D:D, I20)</f>
         <v>47</v>
@@ -17883,11 +17886,6 @@
     <row r="37" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J37" t="s">
         <v>1557</v>
-      </c>
-    </row>
-    <row r="38" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J38" t="s">
-        <v>1560</v>
       </c>
     </row>
   </sheetData>

</xml_diff>